<commit_message>
change presentation and tables
</commit_message>
<xml_diff>
--- a/Algorithm.xlsx
+++ b/Algorithm.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\poshe\OneDrive\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GITHUB\sorting_algorithms\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6968D0E1-49ED-4BF8-9624-7972F92B2E29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B219045-F03A-4506-B1C9-4726F31F9F94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{F93E9351-92C4-45BE-B84E-EDCFF3B27B34}"/>
   </bookViews>
@@ -355,6 +355,21 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="4" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="4" fillId="5" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="4" fillId="6" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -379,21 +394,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="4" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="4" fillId="5" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="4" fillId="6" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -1351,6 +1351,477 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{0000000A-B53E-4339-8217-5255E9CC1C89}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="6"/>
+          <c:order val="6"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Лист1!$I$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Bubble Sort</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1">
+                    <a:lumMod val="60000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="ru-BY"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="r"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Лист1!$J$2:$N$2</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>250000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Лист1!$J$3:$N$3</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7.666666666666667</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>401.66666666666669</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16315.333333333334</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>183766.33333333334</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-5515-4F3D-B1B5-1062EC65F5A2}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="7"/>
+          <c:order val="7"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Лист1!$I$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Insertion Sort</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2">
+                    <a:lumMod val="60000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="ru-BY"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="r"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Лист1!$J$2:$N$2</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>250000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Лист1!$J$4:$N$4</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.6666666666666667</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>16.666666666666668</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1010.3333333333334</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6336</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-5515-4F3D-B1B5-1062EC65F5A2}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="8"/>
+          <c:order val="8"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Лист1!$I$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Selection Sort</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3">
+                    <a:lumMod val="60000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="ru-BY"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="r"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Лист1!$J$2:$N$2</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>250000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Лист1!$J$5:$N$5</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>59.333333333333336</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5780</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>40926.333333333336</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-5515-4F3D-B1B5-1062EC65F5A2}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2610,8 +3081,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C2009DF-69C8-4C2D-966F-0726D8C76FF1}">
   <dimension ref="A1:N35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2:N12"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="Y23" sqref="Y23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="18" x14ac:dyDescent="0.35"/>
@@ -2626,21 +3097,21 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A1" s="2"/>
-      <c r="B1" s="34" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="35"/>
-      <c r="D1" s="35"/>
-      <c r="E1" s="35"/>
-      <c r="F1" s="36"/>
-      <c r="I1" s="32" t="s">
+      <c r="B1" s="43" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="44"/>
+      <c r="D1" s="44"/>
+      <c r="E1" s="44"/>
+      <c r="F1" s="45"/>
+      <c r="I1" s="41" t="s">
         <v>15</v>
       </c>
-      <c r="J1" s="33"/>
-      <c r="K1" s="33"/>
-      <c r="L1" s="33"/>
-      <c r="M1" s="33"/>
-      <c r="N1" s="33"/>
+      <c r="J1" s="42"/>
+      <c r="K1" s="42"/>
+      <c r="L1" s="42"/>
+      <c r="M1" s="42"/>
+      <c r="N1" s="42"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
@@ -2679,34 +3150,34 @@
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A3" s="37" t="s">
+      <c r="A3" s="46" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="31"/>
-      <c r="C3" s="31"/>
-      <c r="D3" s="31"/>
-      <c r="E3" s="31"/>
-      <c r="F3" s="31"/>
-      <c r="I3" s="38" t="s">
+      <c r="B3" s="40"/>
+      <c r="C3" s="40"/>
+      <c r="D3" s="40"/>
+      <c r="E3" s="40"/>
+      <c r="F3" s="40"/>
+      <c r="I3" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="J3" s="39">
+      <c r="J3" s="31">
         <f t="shared" ref="J3:J12" si="0">AVERAGE(B4,B15,B26)</f>
         <v>0</v>
       </c>
-      <c r="K3" s="39">
+      <c r="K3" s="31">
         <f t="shared" ref="K3:K12" si="1">AVERAGE(C4,C15,C26)</f>
         <v>7.666666666666667</v>
       </c>
-      <c r="L3" s="39">
+      <c r="L3" s="31">
         <f t="shared" ref="L3:L12" si="2">AVERAGE(D4,D15,D26)</f>
         <v>401.66666666666669</v>
       </c>
-      <c r="M3" s="39">
+      <c r="M3" s="31">
         <f t="shared" ref="M3:M12" si="3">AVERAGE(E4,E15,E26)</f>
         <v>16315.333333333334</v>
       </c>
-      <c r="N3" s="40">
+      <c r="N3" s="32">
         <f t="shared" ref="N3:N12" si="4">AVERAGE(F4,F15,F26)</f>
         <v>183766.33333333334</v>
       </c>
@@ -2730,26 +3201,26 @@
       <c r="F4" s="25">
         <v>201433</v>
       </c>
-      <c r="I4" s="44" t="s">
+      <c r="I4" s="36" t="s">
         <v>2</v>
       </c>
-      <c r="J4" s="45">
+      <c r="J4" s="37">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K4" s="45">
+      <c r="K4" s="37">
         <f t="shared" si="1"/>
         <v>1.6666666666666667</v>
       </c>
-      <c r="L4" s="45">
+      <c r="L4" s="37">
         <f t="shared" si="2"/>
         <v>16.666666666666668</v>
       </c>
-      <c r="M4" s="45">
+      <c r="M4" s="37">
         <f t="shared" si="3"/>
         <v>1010.3333333333334</v>
       </c>
-      <c r="N4" s="46">
+      <c r="N4" s="38">
         <f t="shared" si="4"/>
         <v>6336</v>
       </c>
@@ -2773,26 +3244,26 @@
       <c r="F5" s="10">
         <v>6067</v>
       </c>
-      <c r="I5" s="41" t="s">
+      <c r="I5" s="33" t="s">
         <v>3</v>
       </c>
-      <c r="J5" s="42">
+      <c r="J5" s="34">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K5" s="42">
+      <c r="K5" s="34">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="L5" s="42">
+      <c r="L5" s="34">
         <f t="shared" si="2"/>
         <v>59.333333333333336</v>
       </c>
-      <c r="M5" s="42">
+      <c r="M5" s="34">
         <f t="shared" si="3"/>
         <v>5780</v>
       </c>
-      <c r="N5" s="43">
+      <c r="N5" s="35">
         <f t="shared" si="4"/>
         <v>40926.333333333336</v>
       </c>
@@ -3119,14 +3590,14 @@
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A14" s="30" t="s">
+      <c r="A14" s="39" t="s">
         <v>12</v>
       </c>
-      <c r="B14" s="31"/>
-      <c r="C14" s="31"/>
-      <c r="D14" s="31"/>
-      <c r="E14" s="31"/>
-      <c r="F14" s="31"/>
+      <c r="B14" s="40"/>
+      <c r="C14" s="40"/>
+      <c r="D14" s="40"/>
+      <c r="E14" s="40"/>
+      <c r="F14" s="40"/>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A15" s="6" t="s">
@@ -3329,14 +3800,14 @@
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A25" s="30" t="s">
+      <c r="A25" s="39" t="s">
         <v>13</v>
       </c>
-      <c r="B25" s="31"/>
-      <c r="C25" s="31"/>
-      <c r="D25" s="31"/>
-      <c r="E25" s="31"/>
-      <c r="F25" s="31"/>
+      <c r="B25" s="40"/>
+      <c r="C25" s="40"/>
+      <c r="D25" s="40"/>
+      <c r="E25" s="40"/>
+      <c r="F25" s="40"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A26" s="6" t="s">

</xml_diff>